<commit_message>
Add three plots to ICS work
Ratio of ICS account balance to the DCP obligation at two different Lake Mead water levels. DCP obligations increase as the Lake Mead level falls. This ratio is the number of years water in the ICS account could cover the DCP obligation.

Ratio of the ICS withdrawal limit to the DCP obligation at two different Lake Mead water levels. If ICS withdrawal limits are enforced, this ratio represents the fraction of the DCP obligation the state could pay from previously conserved water (in the ICS account)

Ratio of the ICS deposit limit to the DCP obligation at two different Lake Mead water levels. If deposit limits are enforced, this ratio shows how well a state can keep up year-to-year with its DCP obligations by conserving and adding water to it's ICS account.
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24C01D3-FF84-4365-8D64-39C42A0071CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DEC454-308E-40FD-9E86-B8EA329CB2C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="By User" sheetId="2" r:id="rId2"/>
+    <sheet name="ICStoDCP" sheetId="3" r:id="rId2"/>
+    <sheet name="By User" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="52">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -152,15 +153,46 @@
   </si>
   <si>
     <t>Balance - Dec 2019 (AF)</t>
+  </si>
+  <si>
+    <t>DCP-AZ Reduction (ac-ft)</t>
+  </si>
+  <si>
+    <t>DCP-NV Reduction (ac-ft)</t>
+  </si>
+  <si>
+    <t>DCP-CA Reduction (ac-ft)</t>
+  </si>
+  <si>
+    <t>Mead Elevation (ft)</t>
+  </si>
+  <si>
+    <t>Years ICS can convert to DCP</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>Percent of DCP obligation ICS max withdrawal can meet</t>
+  </si>
+  <si>
+    <t>Percent of DCP obliation max ICS deposit can fund</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -186,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,8 +231,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -223,12 +261,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -251,18 +299,33 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -542,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,10 +683,10 @@
         <f>SUM(B7:D7)</f>
         <v>2312627</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>2019</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <f>E7-E8</f>
         <v>570695</v>
       </c>
@@ -651,7 +714,7 @@
       <c r="F8" s="10">
         <v>2018</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <f>E8-E9</f>
         <v>480441</v>
       </c>
@@ -679,7 +742,7 @@
       <c r="F9" s="11">
         <v>2017</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <f t="shared" ref="G9:G15" si="0">E9-E10</f>
         <v>511813</v>
       </c>
@@ -710,7 +773,7 @@
       <c r="F10" s="11">
         <v>2016</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <f t="shared" si="0"/>
         <v>37814</v>
       </c>
@@ -738,7 +801,7 @@
       <c r="F11" s="11">
         <v>2015</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="12">
         <f t="shared" si="0"/>
         <v>-125036</v>
       </c>
@@ -766,7 +829,7 @@
       <c r="F12" s="11">
         <v>2014</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="12">
         <f t="shared" si="0"/>
         <v>-281264</v>
       </c>
@@ -794,7 +857,7 @@
       <c r="F13" s="11">
         <v>2013</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <f t="shared" si="0"/>
         <v>-77476</v>
       </c>
@@ -822,7 +885,7 @@
       <c r="F14" s="11">
         <v>2012</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <f t="shared" si="0"/>
         <v>169240</v>
       </c>
@@ -850,7 +913,7 @@
       <c r="F15" s="11">
         <v>2011</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="12">
         <f t="shared" si="0"/>
         <v>211059</v>
       </c>
@@ -878,7 +941,7 @@
       <c r="F16" s="11">
         <v>2010</v>
       </c>
-      <c r="G16" s="13"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -1028,13 +1091,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -1093,11 +1156,487 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="16">
+        <v>1218.5</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="16">
+        <v>1190</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="16">
+        <v>1150</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>1091</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>1090</v>
+      </c>
+      <c r="B7" s="7">
+        <v>192000</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7">
+        <v>8000</v>
+      </c>
+      <c r="E7" s="17">
+        <f>Sheet1!B$7/B7</f>
+        <v>2.4661666666666666</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17">
+        <f>Sheet1!D$7/D7</f>
+        <v>98.239125000000001</v>
+      </c>
+      <c r="H7" s="19">
+        <f>Sheet1!B$25/ICStoDCP!B7</f>
+        <v>1.5625</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19">
+        <f>Sheet1!D$25/ICStoDCP!D7</f>
+        <v>37.5</v>
+      </c>
+      <c r="K7" s="18">
+        <f>Sheet1!B$23/ICStoDCP!B7</f>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18">
+        <f>Sheet1!D$23/ICStoDCP!D7</f>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>1075</v>
+      </c>
+      <c r="B8" s="7">
+        <v>512000</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7">
+        <v>21000</v>
+      </c>
+      <c r="E8" s="17">
+        <f>Sheet1!B$7/B8</f>
+        <v>0.92481250000000004</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17">
+        <f>Sheet1!D$7/D8</f>
+        <v>37.424428571428571</v>
+      </c>
+      <c r="H8" s="19">
+        <f>Sheet1!B$25/ICStoDCP!B8</f>
+        <v>0.5859375</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19">
+        <f>Sheet1!D$25/ICStoDCP!D8</f>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="K8" s="18">
+        <f>Sheet1!B$23/ICStoDCP!B8</f>
+        <v>0.1953125</v>
+      </c>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18">
+        <f>Sheet1!D$23/ICStoDCP!D8</f>
+        <v>5.9523809523809526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
+        <v>1050</v>
+      </c>
+      <c r="B9" s="7">
+        <v>592000</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7">
+        <v>25000</v>
+      </c>
+      <c r="E9" s="17">
+        <f>Sheet1!B$7/B9</f>
+        <v>0.7998378378378378</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17">
+        <f>Sheet1!D$7/D9</f>
+        <v>31.436520000000002</v>
+      </c>
+      <c r="H9" s="19">
+        <f>Sheet1!B$25/ICStoDCP!B9</f>
+        <v>0.5067567567567568</v>
+      </c>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19">
+        <f>Sheet1!D$25/ICStoDCP!D9</f>
+        <v>12</v>
+      </c>
+      <c r="K9" s="18">
+        <f>Sheet1!B$23/ICStoDCP!B9</f>
+        <v>0.16891891891891891</v>
+      </c>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18">
+        <f>Sheet1!D$23/ICStoDCP!D9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <v>1045</v>
+      </c>
+      <c r="B10" s="7">
+        <v>640000</v>
+      </c>
+      <c r="C10" s="7">
+        <v>200000</v>
+      </c>
+      <c r="D10" s="7">
+        <v>27000</v>
+      </c>
+      <c r="E10" s="17">
+        <f>Sheet1!B$7/B10</f>
+        <v>0.73985000000000001</v>
+      </c>
+      <c r="F10" s="17">
+        <f>Sheet1!C$7/C10</f>
+        <v>5.2660499999999999</v>
+      </c>
+      <c r="G10" s="17">
+        <f>Sheet1!D$7/D10</f>
+        <v>29.10788888888889</v>
+      </c>
+      <c r="H10" s="19">
+        <f>Sheet1!B$25/ICStoDCP!B10</f>
+        <v>0.46875</v>
+      </c>
+      <c r="I10" s="19">
+        <f>Sheet1!C$25/ICStoDCP!C10</f>
+        <v>2</v>
+      </c>
+      <c r="J10" s="19">
+        <f>Sheet1!D$25/ICStoDCP!D10</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="K10" s="18">
+        <f>Sheet1!B$23/ICStoDCP!B10</f>
+        <v>0.15625</v>
+      </c>
+      <c r="L10" s="18">
+        <f>Sheet1!C$23/ICStoDCP!C10</f>
+        <v>2</v>
+      </c>
+      <c r="M10" s="18">
+        <f>Sheet1!D$23/ICStoDCP!D10</f>
+        <v>4.6296296296296298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>1040</v>
+      </c>
+      <c r="B11" s="7">
+        <v>640000</v>
+      </c>
+      <c r="C11" s="7">
+        <v>250000</v>
+      </c>
+      <c r="D11" s="7">
+        <v>27000</v>
+      </c>
+      <c r="E11" s="17">
+        <f>Sheet1!B$7/B11</f>
+        <v>0.73985000000000001</v>
+      </c>
+      <c r="F11" s="17">
+        <f>Sheet1!C$7/C11</f>
+        <v>4.2128399999999999</v>
+      </c>
+      <c r="G11" s="17">
+        <f>Sheet1!D$7/D11</f>
+        <v>29.10788888888889</v>
+      </c>
+      <c r="H11" s="19">
+        <f>Sheet1!B$25/ICStoDCP!B11</f>
+        <v>0.46875</v>
+      </c>
+      <c r="I11" s="19">
+        <f>Sheet1!C$25/ICStoDCP!C11</f>
+        <v>1.6</v>
+      </c>
+      <c r="J11" s="19">
+        <f>Sheet1!D$25/ICStoDCP!D11</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="K11" s="18">
+        <f>Sheet1!B$23/ICStoDCP!B11</f>
+        <v>0.15625</v>
+      </c>
+      <c r="L11" s="18">
+        <f>Sheet1!C$23/ICStoDCP!C11</f>
+        <v>1.6</v>
+      </c>
+      <c r="M11" s="18">
+        <f>Sheet1!D$23/ICStoDCP!D11</f>
+        <v>4.6296296296296298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>1035</v>
+      </c>
+      <c r="B12" s="7">
+        <v>640000</v>
+      </c>
+      <c r="C12" s="7">
+        <v>300000</v>
+      </c>
+      <c r="D12" s="7">
+        <v>27000</v>
+      </c>
+      <c r="E12" s="17">
+        <f>Sheet1!B$7/B12</f>
+        <v>0.73985000000000001</v>
+      </c>
+      <c r="F12" s="17">
+        <f>Sheet1!C$7/C12</f>
+        <v>3.5106999999999999</v>
+      </c>
+      <c r="G12" s="17">
+        <f>Sheet1!D$7/D12</f>
+        <v>29.10788888888889</v>
+      </c>
+      <c r="H12" s="19">
+        <f>Sheet1!B$25/ICStoDCP!B12</f>
+        <v>0.46875</v>
+      </c>
+      <c r="I12" s="19">
+        <f>Sheet1!C$25/ICStoDCP!C12</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J12" s="19">
+        <f>Sheet1!D$25/ICStoDCP!D12</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="K12" s="18">
+        <f>Sheet1!B$23/ICStoDCP!B12</f>
+        <v>0.15625</v>
+      </c>
+      <c r="L12" s="18">
+        <f>Sheet1!C$23/ICStoDCP!C12</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="M12" s="18">
+        <f>Sheet1!D$23/ICStoDCP!D12</f>
+        <v>4.6296296296296298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>1030</v>
+      </c>
+      <c r="B13" s="7">
+        <v>640000</v>
+      </c>
+      <c r="C13" s="7">
+        <v>350000</v>
+      </c>
+      <c r="D13" s="7">
+        <v>27000</v>
+      </c>
+      <c r="E13" s="17">
+        <f>Sheet1!B$7/B13</f>
+        <v>0.73985000000000001</v>
+      </c>
+      <c r="F13" s="17">
+        <f>Sheet1!C$7/C13</f>
+        <v>3.0091714285714284</v>
+      </c>
+      <c r="G13" s="17">
+        <f>Sheet1!D$7/D13</f>
+        <v>29.10788888888889</v>
+      </c>
+      <c r="H13" s="19">
+        <f>Sheet1!B$25/ICStoDCP!B13</f>
+        <v>0.46875</v>
+      </c>
+      <c r="I13" s="19">
+        <f>Sheet1!C$25/ICStoDCP!C13</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="J13" s="19">
+        <f>Sheet1!D$25/ICStoDCP!D13</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="K13" s="18">
+        <f>Sheet1!B$23/ICStoDCP!B13</f>
+        <v>0.15625</v>
+      </c>
+      <c r="L13" s="18">
+        <f>Sheet1!C$23/ICStoDCP!C13</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="M13" s="18">
+        <f>Sheet1!D$23/ICStoDCP!D13</f>
+        <v>4.6296296296296298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>1025</v>
+      </c>
+      <c r="B14" s="7">
+        <v>720000</v>
+      </c>
+      <c r="C14" s="7">
+        <v>350000</v>
+      </c>
+      <c r="D14" s="7">
+        <v>30000</v>
+      </c>
+      <c r="E14" s="17">
+        <f>Sheet1!B$7/B14</f>
+        <v>0.65764444444444448</v>
+      </c>
+      <c r="F14" s="17">
+        <f>Sheet1!C$7/C14</f>
+        <v>3.0091714285714284</v>
+      </c>
+      <c r="G14" s="17">
+        <f>Sheet1!D$7/D14</f>
+        <v>26.197099999999999</v>
+      </c>
+      <c r="H14" s="19">
+        <f>Sheet1!B$25/ICStoDCP!B14</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I14" s="19">
+        <f>Sheet1!C$25/ICStoDCP!C14</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="J14" s="19">
+        <f>Sheet1!D$25/ICStoDCP!D14</f>
+        <v>10</v>
+      </c>
+      <c r="K14" s="18">
+        <f>Sheet1!B$23/ICStoDCP!B14</f>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="L14" s="18">
+        <f>Sheet1!C$23/ICStoDCP!C14</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="M14" s="18">
+        <f>Sheet1!D$23/ICStoDCP!D14</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1240,7 +1779,7 @@
         <f>19798+28566+799+400000+2094</f>
         <v>451257</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1300,7 +1839,7 @@
         <f>77162+29870+2722+400000+3050</f>
         <v>512804</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">

</xml_diff>

<commit_message>
Add Lake Mead to interactive water budget role play
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E97B61C-5A4E-40BB-9EFB-CA76575D1B21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D27C643-0E22-4343-BD1B-AE080F922BD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="51">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Each subsequent year</t>
   </si>
   <si>
-    <t>Why is NV greater than Max Total?</t>
-  </si>
-  <si>
     <t>ICS reduced when reservoir flood control releases made.</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Difference</t>
-  </si>
-  <si>
     <t>Balance - Dec 2014 (AF)</t>
   </si>
   <si>
@@ -183,6 +177,9 @@
   </si>
   <si>
     <t>Percent of DCP obliation max ICS deposit can fund</t>
+  </si>
+  <si>
+    <t>Annual Addition</t>
   </si>
 </sst>
 </file>
@@ -276,7 +273,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -319,6 +316,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,29 +619,38 @@
     <col min="5" max="5" width="10.36328125" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -657,15 +667,24 @@
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F7,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -690,10 +709,22 @@
         <f>E7-E8</f>
         <v>570695</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="22">
+        <f>B7-B8</f>
+        <v>130452</v>
+      </c>
+      <c r="I7" s="22">
+        <f t="shared" ref="I7:J7" si="0">C7-C8</f>
+        <v>354778</v>
+      </c>
+      <c r="J7" s="22">
+        <f t="shared" si="0"/>
+        <v>85465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F8,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -718,8 +749,20 @@
         <f>E8-E9</f>
         <v>480441</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H8" s="22">
+        <f t="shared" ref="H8:H15" si="1">B8-B9</f>
+        <v>216252</v>
+      </c>
+      <c r="I8" s="22">
+        <f t="shared" ref="I8:I15" si="2">C8-C9</f>
+        <v>146054</v>
+      </c>
+      <c r="J8" s="22">
+        <f t="shared" ref="J8:J15" si="3">D8-D9</f>
+        <v>118135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -743,14 +786,23 @@
         <v>2017</v>
       </c>
       <c r="G9" s="12">
-        <f t="shared" ref="G9:G15" si="0">E9-E10</f>
+        <f t="shared" ref="G9:G15" si="4">E9-E10</f>
         <v>511813</v>
       </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H9" s="22">
+        <f t="shared" si="1"/>
+        <v>23750</v>
+      </c>
+      <c r="I9" s="22">
+        <f t="shared" si="2"/>
+        <v>437312</v>
+      </c>
+      <c r="J9" s="22">
+        <f t="shared" si="3"/>
+        <v>50751</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -767,18 +819,30 @@
         <v>531562</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" ref="E10:E16" si="1">SUM(B10:D10)</f>
+        <f t="shared" ref="E10:E16" si="5">SUM(B10:D10)</f>
         <v>749678</v>
       </c>
       <c r="F10" s="11">
         <v>2016</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>37814</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H10" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="22">
+        <f t="shared" si="2"/>
+        <v>17275</v>
+      </c>
+      <c r="J10" s="22">
+        <f t="shared" si="3"/>
+        <v>20539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -795,20 +859,32 @@
         <v>511023</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>711864</v>
       </c>
       <c r="F11" s="11">
         <v>2015</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-125036</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H11" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="22">
+        <f t="shared" si="2"/>
+        <v>-71294</v>
+      </c>
+      <c r="J11" s="22">
+        <f t="shared" si="3"/>
+        <v>-53742</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -823,20 +899,32 @@
         <v>564765</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>836900</v>
       </c>
       <c r="F12" s="11">
         <v>2014</v>
       </c>
       <c r="G12" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-281264</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H12" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="22">
+        <f t="shared" si="2"/>
+        <v>-304978</v>
+      </c>
+      <c r="J12" s="22">
+        <f t="shared" si="3"/>
+        <v>23714</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -851,20 +939,32 @@
         <v>541051</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1118164</v>
       </c>
       <c r="F13" s="11">
         <v>2013</v>
       </c>
       <c r="G13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-77476</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H13" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="22">
+        <f t="shared" si="2"/>
+        <v>-105723</v>
+      </c>
+      <c r="J13" s="22">
+        <f t="shared" si="3"/>
+        <v>28247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -879,20 +979,32 @@
         <v>512804</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1195640</v>
       </c>
       <c r="F14" s="11">
         <v>2012</v>
       </c>
       <c r="G14" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>169240</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H14" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="22">
+        <f t="shared" si="2"/>
+        <v>139108</v>
+      </c>
+      <c r="J14" s="22">
+        <f t="shared" si="3"/>
+        <v>30132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -907,20 +1019,32 @@
         <v>482672</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1026400</v>
       </c>
       <c r="F15" s="11">
         <v>2011</v>
       </c>
       <c r="G15" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>211059</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H15" s="22">
+        <f t="shared" si="1"/>
+        <v>956</v>
+      </c>
+      <c r="I15" s="22">
+        <f t="shared" si="2"/>
+        <v>178688</v>
+      </c>
+      <c r="J15" s="22">
+        <f t="shared" si="3"/>
+        <v>31415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -935,7 +1059,7 @@
         <v>451257</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>815341</v>
       </c>
       <c r="F16" s="11">
@@ -957,7 +1081,7 @@
         <v>125000</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" ref="E17:E19" si="2">SUM(B17:D17)</f>
+        <f t="shared" ref="E17:E19" si="6">SUM(B17:D17)</f>
         <v>625000</v>
       </c>
     </row>
@@ -975,7 +1099,7 @@
         <v>300000</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2100000</v>
       </c>
     </row>
@@ -993,13 +1117,13 @@
         <v>300000</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1000000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1014,22 +1138,22 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="9" t="str">
         <f>B6</f>
         <v>Arizona</v>
       </c>
       <c r="C22" s="9" t="str">
-        <f t="shared" ref="C22:E22" si="3">C6</f>
+        <f t="shared" ref="C22:E22" si="7">C6</f>
         <v>California</v>
       </c>
       <c r="D22" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Nevada</v>
       </c>
       <c r="E22" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Total</v>
       </c>
     </row>
@@ -1047,13 +1171,13 @@
         <v>125000</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" ref="E23:E25" si="4">SUM(B23:D23)</f>
+        <f t="shared" ref="E23:E25" si="8">SUM(B23:D23)</f>
         <v>625000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="7">
         <v>500000</v>
@@ -1065,7 +1189,7 @@
         <v>500000</v>
       </c>
       <c r="E24" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2700000</v>
       </c>
     </row>
@@ -1078,21 +1202,21 @@
         <v>300000</v>
       </c>
       <c r="C25" s="7">
-        <f t="shared" ref="C25:D25" si="5">C19</f>
+        <f t="shared" ref="C25:D25" si="9">C19</f>
         <v>400000</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>300000</v>
       </c>
       <c r="E25" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1000000</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -1101,7 +1225,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1148,8 +1272,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1159,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1172,56 +1297,56 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E1" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>49</v>
-      </c>
       <c r="H2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>49</v>
-      </c>
       <c r="K2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1647,16 +1772,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1664,7 +1789,7 @@
         <v>2011</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1681,7 +1806,7 @@
         <v>2011</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1696,7 +1821,7 @@
         <v>2011</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1711,7 +1836,7 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1726,7 +1851,7 @@
         <v>2010</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -1741,7 +1866,7 @@
         <v>2010</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1756,7 +1881,7 @@
         <v>2010</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1770,7 +1895,7 @@
         <v>2010</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1786,7 +1911,7 @@
         <v>2012</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -1801,7 +1926,7 @@
         <v>2012</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1816,7 +1941,7 @@
         <v>2012</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1830,7 +1955,7 @@
         <v>2012</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1846,7 +1971,7 @@
         <v>2013</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1861,7 +1986,7 @@
         <v>2013</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -1876,7 +2001,7 @@
         <v>2013</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1890,7 +2015,7 @@
         <v>2013</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1905,7 +2030,7 @@
         <v>2014</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -1920,7 +2045,7 @@
         <v>2014</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1935,7 +2060,7 @@
         <v>2014</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -1949,7 +2074,7 @@
         <v>2014</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1963,7 +2088,7 @@
         <v>2015</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -1978,7 +2103,7 @@
         <v>2015</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1993,7 +2118,7 @@
         <v>2015</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2007,7 +2132,7 @@
         <v>2015</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -2021,7 +2146,7 @@
         <v>2016</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -2036,7 +2161,7 @@
         <v>2016</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -2051,7 +2176,7 @@
         <v>2016</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -2065,7 +2190,7 @@
         <v>2016</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -2079,7 +2204,7 @@
         <v>2017</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -2093,7 +2218,7 @@
         <v>2017</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -2107,7 +2232,7 @@
         <v>2017</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -2121,7 +2246,7 @@
         <v>2017</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -2135,7 +2260,7 @@
         <v>2018</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -2149,7 +2274,7 @@
         <v>2018</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -2163,7 +2288,7 @@
         <v>2018</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -2177,7 +2302,7 @@
         <v>2018</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -2191,7 +2316,7 @@
         <v>2019</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
@@ -2205,7 +2330,7 @@
         <v>2019</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
@@ -2219,7 +2344,7 @@
         <v>2019</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
@@ -2233,7 +2358,7 @@
         <v>2019</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -2247,7 +2372,7 @@
         <v>2019</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -2261,7 +2386,7 @@
         <v>2019</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update ICS to include 2020 data and new observations
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D27C643-0E22-4343-BD1B-AE080F922BD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906CCA94-EE0F-4340-98D9-A708053D14DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ICStoDCP" sheetId="3" r:id="rId2"/>
-    <sheet name="By User" sheetId="2" r:id="rId3"/>
+    <sheet name="DCPLogs" sheetId="4" r:id="rId3"/>
+    <sheet name="By User" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -180,6 +181,36 @@
   </si>
   <si>
     <t>Annual Addition</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2020 (AF)</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>Required DCP Contribution</t>
+  </si>
+  <si>
+    <t>ConvertExistingICStoDCPICS</t>
+  </si>
+  <si>
+    <t>CreateConvertICStoDCPICS</t>
+  </si>
+  <si>
+    <t>CreatNonICS</t>
+  </si>
+  <si>
+    <t>TotalDCPContribute</t>
+  </si>
+  <si>
+    <t>DCPDeficiency</t>
+  </si>
+  <si>
+    <t>CAWCD</t>
   </si>
 </sst>
 </file>
@@ -273,7 +304,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -312,14 +343,26 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -604,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,42 +658,42 @@
     <col min="1" max="1" width="30.7265625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" customWidth="1"/>
+    <col min="4" max="5" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G5" s="23" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -663,618 +706,696 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L6" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="23">
+        <v>598742</v>
+      </c>
+      <c r="C7" s="23">
+        <v>1375871</v>
+      </c>
+      <c r="D7" s="23">
+        <v>865741</v>
+      </c>
+      <c r="E7" s="23">
+        <f>41000+E8</f>
+        <v>173975</v>
+      </c>
+      <c r="F7" s="2">
+        <f>SUM(B7:D7)</f>
+        <v>2840354</v>
+      </c>
+      <c r="G7" s="24">
+        <v>2020</v>
+      </c>
+      <c r="H7" s="12">
+        <f>F7-F8</f>
+        <v>527727</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" ref="I7:L8" si="0">B7-B8</f>
+        <v>125238</v>
+      </c>
+      <c r="J7" s="20">
+        <f t="shared" si="0"/>
+        <v>322661</v>
+      </c>
+      <c r="K7" s="20">
+        <f t="shared" si="0"/>
+        <v>79828</v>
+      </c>
+      <c r="L7" s="20">
+        <f t="shared" si="0"/>
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F7,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>473504</v>
       </c>
-      <c r="C7" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F7,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>1053210</v>
       </c>
-      <c r="D7" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F7,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>785913</v>
       </c>
-      <c r="E7" s="2">
-        <f>SUM(B7:D7)</f>
+      <c r="E8" s="2">
+        <v>132975</v>
+      </c>
+      <c r="F8" s="2">
+        <f>SUM(B8:D8)</f>
         <v>2312627</v>
       </c>
-      <c r="F7" s="14">
+      <c r="G8" s="14">
         <v>2019</v>
       </c>
-      <c r="G7" s="12">
-        <f>E7-E8</f>
+      <c r="H8" s="12">
+        <f>F8-F9</f>
         <v>570695</v>
       </c>
-      <c r="H7" s="22">
-        <f>B7-B8</f>
+      <c r="I8" s="20">
+        <f t="shared" si="0"/>
         <v>130452</v>
       </c>
-      <c r="I7" s="22">
-        <f t="shared" ref="I7:J7" si="0">C7-C8</f>
+      <c r="J8" s="20">
+        <f t="shared" si="0"/>
         <v>354778</v>
       </c>
-      <c r="J7" s="22">
+      <c r="K8" s="20">
         <f t="shared" si="0"/>
         <v>85465</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F8,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>343052</v>
       </c>
-      <c r="C8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F8,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>698432</v>
       </c>
-      <c r="D8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F8,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>700448</v>
       </c>
-      <c r="E8" s="2">
-        <f>SUM(B8:D8)</f>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <f>SUM(B9:D9)</f>
         <v>1741932</v>
       </c>
-      <c r="F8" s="10">
+      <c r="G9" s="10">
         <v>2018</v>
       </c>
-      <c r="G8" s="12">
-        <f>E8-E9</f>
+      <c r="H9" s="12">
+        <f>F9-F10</f>
         <v>480441</v>
       </c>
-      <c r="H8" s="22">
-        <f t="shared" ref="H8:H15" si="1">B8-B9</f>
+      <c r="I9" s="20">
+        <f t="shared" ref="I9:I16" si="1">B9-B10</f>
         <v>216252</v>
       </c>
-      <c r="I8" s="22">
-        <f t="shared" ref="I8:I15" si="2">C8-C9</f>
+      <c r="J9" s="20">
+        <f t="shared" ref="J9:J16" si="2">C9-C10</f>
         <v>146054</v>
       </c>
-      <c r="J8" s="22">
-        <f t="shared" ref="J8:J15" si="3">D8-D9</f>
+      <c r="K9" s="20">
+        <f t="shared" ref="K9:K16" si="3">D9-D10</f>
         <v>118135</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F9,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>126800</v>
       </c>
-      <c r="C9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F9,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>552378</v>
       </c>
-      <c r="D9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F9,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>582313</v>
       </c>
-      <c r="E9" s="2">
-        <f>SUM(B9:D9)</f>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <f>SUM(B10:D10)</f>
         <v>1261491</v>
       </c>
-      <c r="F9" s="11">
+      <c r="G10" s="11">
         <v>2017</v>
       </c>
-      <c r="G9" s="12">
-        <f t="shared" ref="G9:G15" si="4">E9-E10</f>
+      <c r="H10" s="12">
+        <f t="shared" ref="H10:H16" si="4">F10-F11</f>
         <v>511813</v>
       </c>
-      <c r="H9" s="22">
+      <c r="I10" s="20">
         <f t="shared" si="1"/>
         <v>23750</v>
       </c>
-      <c r="I9" s="22">
+      <c r="J10" s="20">
         <f t="shared" si="2"/>
         <v>437312</v>
       </c>
-      <c r="J9" s="22">
+      <c r="K10" s="20">
         <f t="shared" si="3"/>
         <v>50751</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F10,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>103050</v>
       </c>
-      <c r="C10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F10,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>115066</v>
       </c>
-      <c r="D10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F10,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>531562</v>
       </c>
-      <c r="E10" s="2">
-        <f t="shared" ref="E10:E16" si="5">SUM(B10:D10)</f>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <f t="shared" ref="F11:F17" si="5">SUM(B11:D11)</f>
         <v>749678</v>
       </c>
-      <c r="F10" s="11">
+      <c r="G11" s="11">
         <v>2016</v>
       </c>
-      <c r="G10" s="12">
+      <c r="H11" s="12">
         <f t="shared" si="4"/>
         <v>37814</v>
       </c>
-      <c r="H10" s="22">
+      <c r="I11" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="22">
+      <c r="J11" s="20">
         <f t="shared" si="2"/>
         <v>17275</v>
       </c>
-      <c r="J10" s="22">
+      <c r="K11" s="20">
         <f t="shared" si="3"/>
         <v>20539</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F11,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B12" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>103050</v>
       </c>
-      <c r="C11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F11,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C12" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>97791</v>
       </c>
-      <c r="D11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F11,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D12" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>511023</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
         <f t="shared" si="5"/>
         <v>711864</v>
       </c>
-      <c r="F11" s="11">
+      <c r="G12" s="11">
         <v>2015</v>
       </c>
-      <c r="G11" s="12">
+      <c r="H12" s="12">
         <f t="shared" si="4"/>
         <v>-125036</v>
       </c>
-      <c r="H11" s="22">
+      <c r="I12" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="22">
+      <c r="J12" s="20">
         <f t="shared" si="2"/>
         <v>-71294</v>
       </c>
-      <c r="J11" s="22">
+      <c r="K12" s="20">
         <f t="shared" si="3"/>
         <v>-53742</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B13" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>103050</v>
       </c>
-      <c r="C12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F12,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C13" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>169085</v>
       </c>
-      <c r="D12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F12,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D13" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>564765</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
         <f t="shared" si="5"/>
         <v>836900</v>
       </c>
-      <c r="F12" s="11">
+      <c r="G13" s="11">
         <v>2014</v>
       </c>
-      <c r="G12" s="12">
+      <c r="H13" s="12">
         <f t="shared" si="4"/>
         <v>-281264</v>
       </c>
-      <c r="H12" s="22">
+      <c r="I13" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="22">
+      <c r="J13" s="20">
         <f t="shared" si="2"/>
         <v>-304978</v>
       </c>
-      <c r="J12" s="22">
+      <c r="K13" s="20">
         <f t="shared" si="3"/>
         <v>23714</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>103050</v>
       </c>
-      <c r="C13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F13,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>474063</v>
       </c>
-      <c r="D13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F13,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>541051</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
         <f t="shared" si="5"/>
         <v>1118164</v>
       </c>
-      <c r="F13" s="11">
+      <c r="G14" s="11">
         <v>2013</v>
       </c>
-      <c r="G13" s="12">
+      <c r="H14" s="12">
         <f t="shared" si="4"/>
         <v>-77476</v>
       </c>
-      <c r="H13" s="22">
+      <c r="I14" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" s="22">
+      <c r="J14" s="20">
         <f t="shared" si="2"/>
         <v>-105723</v>
       </c>
-      <c r="J13" s="22">
+      <c r="K14" s="20">
         <f t="shared" si="3"/>
         <v>28247</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B15" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>103050</v>
       </c>
-      <c r="C14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F14,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C15" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>579786</v>
       </c>
-      <c r="D14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F14,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D15" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>512804</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
         <f t="shared" si="5"/>
         <v>1195640</v>
       </c>
-      <c r="F14" s="11">
+      <c r="G15" s="11">
         <v>2012</v>
       </c>
-      <c r="G14" s="12">
+      <c r="H15" s="12">
         <f t="shared" si="4"/>
         <v>169240</v>
       </c>
-      <c r="H14" s="22">
+      <c r="I15" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" s="22">
+      <c r="J15" s="20">
         <f t="shared" si="2"/>
         <v>139108</v>
       </c>
-      <c r="J14" s="22">
+      <c r="K15" s="20">
         <f t="shared" si="3"/>
         <v>30132</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B16" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>103050</v>
       </c>
-      <c r="C15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F15,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C16" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>440678</v>
       </c>
-      <c r="D15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F15,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D16" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>482672</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
         <f t="shared" si="5"/>
         <v>1026400</v>
       </c>
-      <c r="F15" s="11">
+      <c r="G16" s="11">
         <v>2011</v>
       </c>
-      <c r="G15" s="12">
+      <c r="H16" s="12">
         <f t="shared" si="4"/>
         <v>211059</v>
       </c>
-      <c r="H15" s="22">
+      <c r="I16" s="20">
         <f t="shared" si="1"/>
         <v>956</v>
       </c>
-      <c r="I15" s="22">
+      <c r="J16" s="20">
         <f t="shared" si="2"/>
         <v>178688</v>
       </c>
-      <c r="J15" s="22">
+      <c r="K16" s="20">
         <f t="shared" si="3"/>
         <v>31415</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+      <c r="B17" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>102094</v>
       </c>
-      <c r="C16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F16,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+      <c r="C17" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>261990</v>
       </c>
-      <c r="D16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F16,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+      <c r="D17" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>451257</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
         <f t="shared" si="5"/>
         <v>815341</v>
       </c>
-      <c r="F16" s="11">
+      <c r="G17" s="11">
         <v>2010</v>
       </c>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="2">
         <v>100000</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="2">
         <v>400000</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>125000</v>
       </c>
-      <c r="E17" s="2">
-        <f t="shared" ref="E17:E19" si="6">SUM(B17:D17)</f>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
+        <f t="shared" ref="F18:F20" si="6">SUM(B18:D18)</f>
         <v>625000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <v>300000</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <v>1500000</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <v>300000</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
         <f t="shared" si="6"/>
         <v>2100000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="2">
         <v>300000</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C20" s="2">
         <v>400000</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <v>300000</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
         <f t="shared" si="6"/>
         <v>1000000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="9" t="str">
+      <c r="B23" s="9" t="str">
         <f>B6</f>
         <v>Arizona</v>
       </c>
-      <c r="C22" s="9" t="str">
-        <f t="shared" ref="C22:E22" si="7">C6</f>
+      <c r="C23" s="9" t="str">
+        <f t="shared" ref="C23:F23" si="7">C6</f>
         <v>California</v>
       </c>
-      <c r="D22" s="9" t="str">
+      <c r="D23" s="9" t="str">
         <f t="shared" si="7"/>
         <v>Nevada</v>
       </c>
-      <c r="E22" s="9" t="str">
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="str">
         <f t="shared" si="7"/>
         <v>Total</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B24" s="7">
         <v>100000</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C24" s="7">
         <v>400000</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D24" s="7">
         <v>125000</v>
       </c>
-      <c r="E23" s="7">
-        <f t="shared" ref="E23:E25" si="8">SUM(B23:D23)</f>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7">
+        <f t="shared" ref="F24:F26" si="8">SUM(B24:D24)</f>
         <v>625000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B25" s="7">
         <v>500000</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C25" s="7">
         <v>1700000</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D25" s="7">
         <v>500000</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E25" s="7"/>
+      <c r="F25" s="7">
         <f t="shared" si="8"/>
         <v>2700000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="7">
-        <f>B19</f>
+      <c r="B26" s="7">
+        <f>B20</f>
         <v>300000</v>
       </c>
-      <c r="C25" s="7">
-        <f t="shared" ref="C25:D25" si="9">C19</f>
+      <c r="C26" s="7">
+        <f t="shared" ref="C26:D26" si="9">C20</f>
         <v>400000</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D26" s="7">
         <f t="shared" si="9"/>
         <v>300000</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E26" s="7"/>
+      <c r="F26" s="7">
         <f t="shared" si="8"/>
         <v>1000000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B31" s="4">
         <v>0.05</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C31" s="4">
         <v>0.05</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D31" s="4">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B32" s="4">
         <v>0.03</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C32" s="4">
         <v>0.03</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D32" s="4">
         <v>0.03</v>
       </c>
+      <c r="E32" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="H5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1285,7 +1406,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1296,11 +1417,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" t="s">
         <v>48</v>
       </c>
@@ -1394,29 +1515,29 @@
       </c>
       <c r="E7" s="17">
         <f>Sheet1!B$7/B7</f>
-        <v>2.4661666666666666</v>
+        <v>3.1184479166666668</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17">
         <f>Sheet1!D$7/D7</f>
-        <v>98.239125000000001</v>
+        <v>108.217625</v>
       </c>
       <c r="H7" s="19">
-        <f>Sheet1!B$25/ICStoDCP!B7</f>
+        <f>Sheet1!B$26/ICStoDCP!B7</f>
         <v>1.5625</v>
       </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19">
-        <f>Sheet1!D$25/ICStoDCP!D7</f>
+        <f>Sheet1!D$26/ICStoDCP!D7</f>
         <v>37.5</v>
       </c>
       <c r="K7" s="18">
-        <f>Sheet1!B$23/ICStoDCP!B7</f>
+        <f>Sheet1!B$24/ICStoDCP!B7</f>
         <v>0.52083333333333337</v>
       </c>
       <c r="L7" s="18"/>
       <c r="M7" s="18">
-        <f>Sheet1!D$23/ICStoDCP!D7</f>
+        <f>Sheet1!D$24/ICStoDCP!D7</f>
         <v>15.625</v>
       </c>
     </row>
@@ -1433,29 +1554,29 @@
       </c>
       <c r="E8" s="17">
         <f>Sheet1!B$7/B8</f>
-        <v>0.92481250000000004</v>
+        <v>1.1694179687499999</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17">
         <f>Sheet1!D$7/D8</f>
-        <v>37.424428571428571</v>
+        <v>41.225761904761903</v>
       </c>
       <c r="H8" s="19">
-        <f>Sheet1!B$25/ICStoDCP!B8</f>
+        <f>Sheet1!B$26/ICStoDCP!B8</f>
         <v>0.5859375</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19">
-        <f>Sheet1!D$25/ICStoDCP!D8</f>
+        <f>Sheet1!D$26/ICStoDCP!D8</f>
         <v>14.285714285714286</v>
       </c>
       <c r="K8" s="18">
-        <f>Sheet1!B$23/ICStoDCP!B8</f>
+        <f>Sheet1!B$24/ICStoDCP!B8</f>
         <v>0.1953125</v>
       </c>
       <c r="L8" s="18"/>
       <c r="M8" s="18">
-        <f>Sheet1!D$23/ICStoDCP!D8</f>
+        <f>Sheet1!D$24/ICStoDCP!D8</f>
         <v>5.9523809523809526</v>
       </c>
     </row>
@@ -1472,29 +1593,29 @@
       </c>
       <c r="E9" s="17">
         <f>Sheet1!B$7/B9</f>
-        <v>0.7998378378378378</v>
+        <v>1.0113885135135134</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17">
         <f>Sheet1!D$7/D9</f>
-        <v>31.436520000000002</v>
+        <v>34.629640000000002</v>
       </c>
       <c r="H9" s="19">
-        <f>Sheet1!B$25/ICStoDCP!B9</f>
+        <f>Sheet1!B$26/ICStoDCP!B9</f>
         <v>0.5067567567567568</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19">
-        <f>Sheet1!D$25/ICStoDCP!D9</f>
+        <f>Sheet1!D$26/ICStoDCP!D9</f>
         <v>12</v>
       </c>
       <c r="K9" s="18">
-        <f>Sheet1!B$23/ICStoDCP!B9</f>
+        <f>Sheet1!B$24/ICStoDCP!B9</f>
         <v>0.16891891891891891</v>
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="18">
-        <f>Sheet1!D$23/ICStoDCP!D9</f>
+        <f>Sheet1!D$24/ICStoDCP!D9</f>
         <v>5</v>
       </c>
     </row>
@@ -1513,38 +1634,38 @@
       </c>
       <c r="E10" s="17">
         <f>Sheet1!B$7/B10</f>
-        <v>0.73985000000000001</v>
+        <v>0.93553437500000003</v>
       </c>
       <c r="F10" s="17">
         <f>Sheet1!C$7/C10</f>
-        <v>5.2660499999999999</v>
+        <v>6.8793550000000003</v>
       </c>
       <c r="G10" s="17">
         <f>Sheet1!D$7/D10</f>
-        <v>29.10788888888889</v>
+        <v>32.064481481481479</v>
       </c>
       <c r="H10" s="19">
-        <f>Sheet1!B$25/ICStoDCP!B10</f>
+        <f>Sheet1!B$26/ICStoDCP!B10</f>
         <v>0.46875</v>
       </c>
       <c r="I10" s="19">
-        <f>Sheet1!C$25/ICStoDCP!C10</f>
+        <f>Sheet1!C$26/ICStoDCP!C10</f>
         <v>2</v>
       </c>
       <c r="J10" s="19">
-        <f>Sheet1!D$25/ICStoDCP!D10</f>
+        <f>Sheet1!D$26/ICStoDCP!D10</f>
         <v>11.111111111111111</v>
       </c>
       <c r="K10" s="18">
-        <f>Sheet1!B$23/ICStoDCP!B10</f>
+        <f>Sheet1!B$24/ICStoDCP!B10</f>
         <v>0.15625</v>
       </c>
       <c r="L10" s="18">
-        <f>Sheet1!C$23/ICStoDCP!C10</f>
+        <f>Sheet1!C$24/ICStoDCP!C10</f>
         <v>2</v>
       </c>
       <c r="M10" s="18">
-        <f>Sheet1!D$23/ICStoDCP!D10</f>
+        <f>Sheet1!D$24/ICStoDCP!D10</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1563,38 +1684,38 @@
       </c>
       <c r="E11" s="17">
         <f>Sheet1!B$7/B11</f>
-        <v>0.73985000000000001</v>
+        <v>0.93553437500000003</v>
       </c>
       <c r="F11" s="17">
         <f>Sheet1!C$7/C11</f>
-        <v>4.2128399999999999</v>
+        <v>5.5034840000000003</v>
       </c>
       <c r="G11" s="17">
         <f>Sheet1!D$7/D11</f>
-        <v>29.10788888888889</v>
+        <v>32.064481481481479</v>
       </c>
       <c r="H11" s="19">
-        <f>Sheet1!B$25/ICStoDCP!B11</f>
+        <f>Sheet1!B$26/ICStoDCP!B11</f>
         <v>0.46875</v>
       </c>
       <c r="I11" s="19">
-        <f>Sheet1!C$25/ICStoDCP!C11</f>
+        <f>Sheet1!C$26/ICStoDCP!C11</f>
         <v>1.6</v>
       </c>
       <c r="J11" s="19">
-        <f>Sheet1!D$25/ICStoDCP!D11</f>
+        <f>Sheet1!D$26/ICStoDCP!D11</f>
         <v>11.111111111111111</v>
       </c>
       <c r="K11" s="18">
-        <f>Sheet1!B$23/ICStoDCP!B11</f>
+        <f>Sheet1!B$24/ICStoDCP!B11</f>
         <v>0.15625</v>
       </c>
       <c r="L11" s="18">
-        <f>Sheet1!C$23/ICStoDCP!C11</f>
+        <f>Sheet1!C$24/ICStoDCP!C11</f>
         <v>1.6</v>
       </c>
       <c r="M11" s="18">
-        <f>Sheet1!D$23/ICStoDCP!D11</f>
+        <f>Sheet1!D$24/ICStoDCP!D11</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1613,38 +1734,38 @@
       </c>
       <c r="E12" s="17">
         <f>Sheet1!B$7/B12</f>
-        <v>0.73985000000000001</v>
+        <v>0.93553437500000003</v>
       </c>
       <c r="F12" s="17">
         <f>Sheet1!C$7/C12</f>
-        <v>3.5106999999999999</v>
+        <v>4.5862366666666663</v>
       </c>
       <c r="G12" s="17">
         <f>Sheet1!D$7/D12</f>
-        <v>29.10788888888889</v>
+        <v>32.064481481481479</v>
       </c>
       <c r="H12" s="19">
-        <f>Sheet1!B$25/ICStoDCP!B12</f>
+        <f>Sheet1!B$26/ICStoDCP!B12</f>
         <v>0.46875</v>
       </c>
       <c r="I12" s="19">
-        <f>Sheet1!C$25/ICStoDCP!C12</f>
+        <f>Sheet1!C$26/ICStoDCP!C12</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="J12" s="19">
-        <f>Sheet1!D$25/ICStoDCP!D12</f>
+        <f>Sheet1!D$26/ICStoDCP!D12</f>
         <v>11.111111111111111</v>
       </c>
       <c r="K12" s="18">
-        <f>Sheet1!B$23/ICStoDCP!B12</f>
+        <f>Sheet1!B$24/ICStoDCP!B12</f>
         <v>0.15625</v>
       </c>
       <c r="L12" s="18">
-        <f>Sheet1!C$23/ICStoDCP!C12</f>
+        <f>Sheet1!C$24/ICStoDCP!C12</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="M12" s="18">
-        <f>Sheet1!D$23/ICStoDCP!D12</f>
+        <f>Sheet1!D$24/ICStoDCP!D12</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1663,38 +1784,38 @@
       </c>
       <c r="E13" s="17">
         <f>Sheet1!B$7/B13</f>
-        <v>0.73985000000000001</v>
+        <v>0.93553437500000003</v>
       </c>
       <c r="F13" s="17">
         <f>Sheet1!C$7/C13</f>
-        <v>3.0091714285714284</v>
+        <v>3.93106</v>
       </c>
       <c r="G13" s="17">
         <f>Sheet1!D$7/D13</f>
-        <v>29.10788888888889</v>
+        <v>32.064481481481479</v>
       </c>
       <c r="H13" s="19">
-        <f>Sheet1!B$25/ICStoDCP!B13</f>
+        <f>Sheet1!B$26/ICStoDCP!B13</f>
         <v>0.46875</v>
       </c>
       <c r="I13" s="19">
-        <f>Sheet1!C$25/ICStoDCP!C13</f>
+        <f>Sheet1!C$26/ICStoDCP!C13</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="J13" s="19">
-        <f>Sheet1!D$25/ICStoDCP!D13</f>
+        <f>Sheet1!D$26/ICStoDCP!D13</f>
         <v>11.111111111111111</v>
       </c>
       <c r="K13" s="18">
-        <f>Sheet1!B$23/ICStoDCP!B13</f>
+        <f>Sheet1!B$24/ICStoDCP!B13</f>
         <v>0.15625</v>
       </c>
       <c r="L13" s="18">
-        <f>Sheet1!C$23/ICStoDCP!C13</f>
+        <f>Sheet1!C$24/ICStoDCP!C13</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="M13" s="18">
-        <f>Sheet1!D$23/ICStoDCP!D13</f>
+        <f>Sheet1!D$24/ICStoDCP!D13</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1713,38 +1834,38 @@
       </c>
       <c r="E14" s="17">
         <f>Sheet1!B$7/B14</f>
-        <v>0.65764444444444448</v>
+        <v>0.83158611111111114</v>
       </c>
       <c r="F14" s="17">
         <f>Sheet1!C$7/C14</f>
-        <v>3.0091714285714284</v>
+        <v>3.93106</v>
       </c>
       <c r="G14" s="17">
         <f>Sheet1!D$7/D14</f>
-        <v>26.197099999999999</v>
+        <v>28.858033333333335</v>
       </c>
       <c r="H14" s="19">
-        <f>Sheet1!B$25/ICStoDCP!B14</f>
+        <f>Sheet1!B$26/ICStoDCP!B14</f>
         <v>0.41666666666666669</v>
       </c>
       <c r="I14" s="19">
-        <f>Sheet1!C$25/ICStoDCP!C14</f>
+        <f>Sheet1!C$26/ICStoDCP!C14</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="J14" s="19">
-        <f>Sheet1!D$25/ICStoDCP!D14</f>
+        <f>Sheet1!D$26/ICStoDCP!D14</f>
         <v>10</v>
       </c>
       <c r="K14" s="18">
-        <f>Sheet1!B$23/ICStoDCP!B14</f>
+        <f>Sheet1!B$24/ICStoDCP!B14</f>
         <v>0.1388888888888889</v>
       </c>
       <c r="L14" s="18">
-        <f>Sheet1!C$23/ICStoDCP!C14</f>
+        <f>Sheet1!C$24/ICStoDCP!C14</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="M14" s="18">
-        <f>Sheet1!D$23/ICStoDCP!D14</f>
+        <f>Sheet1!D$24/ICStoDCP!D14</f>
         <v>4.166666666666667</v>
       </c>
     </row>
@@ -1757,6 +1878,143 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
+  <dimension ref="A2:I5"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="2">
+        <v>192000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>47434</v>
+      </c>
+      <c r="G3" s="2">
+        <v>133174</v>
+      </c>
+      <c r="H3" s="2">
+        <f>SUM(E3:G3)</f>
+        <v>180608</v>
+      </c>
+      <c r="I3" s="2">
+        <f>D3-H3</f>
+        <v>11392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H5" si="0">SUM(E4:G4)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I5" si="1">D4-H4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update DCP totals and blog post drafts
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906CCA94-EE0F-4340-98D9-A708053D14DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64262B94-D747-4A23-9D2F-8D7123F44FA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -665,27 +665,27 @@
     <col min="10" max="10" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="H5" s="26" t="s">
         <v>50</v>
       </c>
@@ -693,7 +693,7 @@
       <c r="J5" s="26"/>
       <c r="K5" s="26"/>
     </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -731,7 +731,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>51</v>
       </c>
@@ -776,7 +776,7 @@
         <v>41000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -819,8 +819,12 @@
         <v>85465</v>
       </c>
       <c r="M8" s="20"/>
-    </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N8" s="20">
+        <f>H8-H7</f>
+        <v>42968</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -861,7 +865,7 @@
         <v>118135</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -902,7 +906,7 @@
         <v>50751</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -943,7 +947,7 @@
         <v>20539</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -984,7 +988,7 @@
         <v>-53742</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1025,7 +1029,7 @@
         <v>23714</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1066,7 +1070,7 @@
         <v>28247</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1107,7 +1111,7 @@
         <v>30132</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1406,7 +1410,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>